<commit_message>
Fix cases, when dataset doesn't need a imputation. Add new results.
</commit_message>
<xml_diff>
--- a/results_expirements/soft_experiments/soft_default/soft_experiments.xlsx
+++ b/results_expirements/soft_experiments/soft_default/soft_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gosha\Desktop\Projects\Improvements-to-ML-algorithms\results_expirements\soft_experiments\soft_default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D1365A-DB86-41AF-BABA-C264305F46FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5F7194-838E-4B3D-A721-5DD2F65B4305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="1392" windowWidth="17064" windowHeight="9468" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17064" windowHeight="9468" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sberbank-russian" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="24">
   <si>
     <t>default (hard)</t>
   </si>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045881CD-FC92-4F68-8616-B3B2A40840F1}">
   <dimension ref="B1:O26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23:O26"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2240,13 +2240,13 @@
         <v>0.16209999999999999</v>
       </c>
       <c r="L9">
-        <v>41429.855100000001</v>
+        <v>41239.968499999901</v>
       </c>
       <c r="M9">
-        <v>28433.039799999999</v>
+        <v>28402.999899999999</v>
       </c>
       <c r="N9">
-        <v>0.87050000000000005</v>
+        <v>0.87170000000000003</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -2275,16 +2275,16 @@
         <v>1857.6</v>
       </c>
       <c r="K10">
-        <v>0.18129999999999999</v>
+        <v>0.1817</v>
       </c>
       <c r="L10">
-        <v>47906.370499999997</v>
+        <v>47882.435299999997</v>
       </c>
       <c r="M10">
-        <v>32148.533899999999</v>
+        <v>32167.810399999998</v>
       </c>
       <c r="N10">
-        <v>0.82669999999999999</v>
+        <v>0.82650000000000001</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -2313,16 +2313,16 @@
         <v>2064</v>
       </c>
       <c r="K11">
-        <v>0.17960000000000001</v>
+        <v>0.18149999999999999</v>
       </c>
       <c r="L11">
-        <v>45898.866399999999</v>
+        <v>46073.158600000002</v>
       </c>
       <c r="M11">
-        <v>31183.451300000001</v>
+        <v>31440.0141999999</v>
       </c>
       <c r="N11">
-        <v>0.8468</v>
+        <v>0.84569999999999901</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -2386,16 +2386,16 @@
         <v>16718.400000000001</v>
       </c>
       <c r="K14">
-        <v>0.16209999999999999</v>
+        <v>0.16170000000000001</v>
       </c>
       <c r="L14">
-        <v>41404.428099999997</v>
+        <v>41297.653599999998</v>
       </c>
       <c r="M14">
-        <v>28424.667199999902</v>
+        <v>28367.798299999999</v>
       </c>
       <c r="N14">
-        <v>0.87080000000000002</v>
+        <v>0.87149999999999905</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -2424,16 +2424,16 @@
         <v>1857.6</v>
       </c>
       <c r="K15">
-        <v>0.18140000000000001</v>
+        <v>0.18060000000000001</v>
       </c>
       <c r="L15">
-        <v>47966.717700000001</v>
+        <v>47902.006800000003</v>
       </c>
       <c r="M15">
-        <v>32190.473699999999</v>
+        <v>32125.017899999901</v>
       </c>
       <c r="N15">
-        <v>0.82599999999999996</v>
+        <v>0.8266</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
@@ -2462,16 +2462,16 @@
         <v>2064</v>
       </c>
       <c r="K16">
-        <v>0.17960000000000001</v>
+        <v>0.17910000000000001</v>
       </c>
       <c r="L16">
-        <v>45834.502599999898</v>
+        <v>45790.553800000002</v>
       </c>
       <c r="M16">
-        <v>31155.1217</v>
+        <v>31117.5</v>
       </c>
       <c r="N16">
-        <v>0.84709999999999996</v>
+        <v>0.84749999999999903</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
@@ -2535,13 +2535,13 @@
         <v>16718.400000000001</v>
       </c>
       <c r="K19">
-        <v>0.16209999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="L19">
-        <v>41421.106599999999</v>
+        <v>41390.044199999997</v>
       </c>
       <c r="M19">
-        <v>28426.952799999999</v>
+        <v>28458.6604999999</v>
       </c>
       <c r="N19">
         <v>0.87070000000000003</v>
@@ -2573,16 +2573,16 @@
         <v>1857.6</v>
       </c>
       <c r="K20">
-        <v>0.18099999999999999</v>
+        <v>0.18149999999999999</v>
       </c>
       <c r="L20">
-        <v>47892.0076999999</v>
+        <v>48039.911899999999</v>
       </c>
       <c r="M20">
-        <v>32122.1891</v>
+        <v>32261.763299999999</v>
       </c>
       <c r="N20">
-        <v>0.82669999999999999</v>
+        <v>0.82549999999999901</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
@@ -2611,16 +2611,16 @@
         <v>2064</v>
       </c>
       <c r="K21">
-        <v>0.1797</v>
+        <v>0.18029999999999899</v>
       </c>
       <c r="L21">
-        <v>45852.187099999901</v>
+        <v>46054.006099999999</v>
       </c>
       <c r="M21">
-        <v>31166.8406</v>
+        <v>31287.5929</v>
       </c>
       <c r="N21">
-        <v>0.84689999999999999</v>
+        <v>0.84570000000000001</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
@@ -2684,16 +2684,16 @@
         <v>16718.400000000001</v>
       </c>
       <c r="K24">
-        <v>0.16209999999999999</v>
+        <v>0.16189999999999999</v>
       </c>
       <c r="L24">
-        <v>41409.956899999997</v>
+        <v>41205.103499999997</v>
       </c>
       <c r="M24">
-        <v>28431.9853999999</v>
+        <v>28393.1611999999</v>
       </c>
       <c r="N24">
-        <v>0.87059999999999904</v>
+        <v>0.87189999999999901</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
@@ -2722,16 +2722,16 @@
         <v>1857.6</v>
       </c>
       <c r="K25">
-        <v>0.18149999999999999</v>
+        <v>0.183699999999999</v>
       </c>
       <c r="L25">
-        <v>47989.002699999997</v>
+        <v>48061.705699999999</v>
       </c>
       <c r="M25">
-        <v>32198.444599999999</v>
+        <v>32379.892699999898</v>
       </c>
       <c r="N25">
-        <v>0.82589999999999997</v>
+        <v>0.82549999999999901</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
@@ -2760,16 +2760,16 @@
         <v>2064</v>
       </c>
       <c r="K26">
-        <v>0.18029999999999999</v>
+        <v>0.18149999999999999</v>
       </c>
       <c r="L26">
-        <v>45994.523999999998</v>
+        <v>45784.567799999997</v>
       </c>
       <c r="M26">
-        <v>31203.5373</v>
+        <v>31323.0281</v>
       </c>
       <c r="N26">
-        <v>0.84609999999999896</v>
+        <v>0.84749999999999903</v>
       </c>
     </row>
   </sheetData>
@@ -3015,16 +3015,16 @@
         <v>3611.7</v>
       </c>
       <c r="K14">
-        <v>4.4359000000000002</v>
+        <v>4.1393000000000004</v>
       </c>
       <c r="L14">
-        <v>3741555.5529999998</v>
+        <v>3666571.86719999</v>
       </c>
       <c r="M14">
-        <v>2426855.6490000002</v>
+        <v>2350293.1891999999</v>
       </c>
       <c r="N14">
-        <v>0.79290000000000005</v>
+        <v>0.801399999999999</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -3053,16 +3053,16 @@
         <v>401.3</v>
       </c>
       <c r="K15">
-        <v>7.9078999999999997</v>
+        <v>7.5333999999999897</v>
       </c>
       <c r="L15">
-        <v>7020595.4819999998</v>
+        <v>6951613.0497000003</v>
       </c>
       <c r="M15">
-        <v>4731939.7439999999</v>
+        <v>4675228.7275999999</v>
       </c>
       <c r="N15">
-        <v>0.26579999999999998</v>
+        <v>0.28059999999999902</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
@@ -3091,16 +3091,16 @@
         <v>446</v>
       </c>
       <c r="K16">
-        <v>6.6943999999999999</v>
+        <v>6.5222999999999898</v>
       </c>
       <c r="L16">
-        <v>7619867.3159999996</v>
+        <v>7577015.1265000002</v>
       </c>
       <c r="M16">
-        <v>5103355.6040000003</v>
+        <v>5035427.2412</v>
       </c>
       <c r="N16">
-        <v>0.16189999999999999</v>
+        <v>0.1714</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
@@ -3164,16 +3164,16 @@
         <v>3611.7</v>
       </c>
       <c r="K19">
-        <v>4.5415000000000001</v>
+        <v>4.4104999999999999</v>
       </c>
       <c r="L19">
-        <v>3775938.2785</v>
+        <v>3725080.2409999999</v>
       </c>
       <c r="M19">
-        <v>2434391.25</v>
+        <v>2414190.0791000002</v>
       </c>
       <c r="N19">
-        <v>0.78910000000000002</v>
+        <v>0.79490000000000005</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
@@ -3202,16 +3202,16 @@
         <v>401.3</v>
       </c>
       <c r="K20">
-        <v>7.87889999999999</v>
+        <v>7.7874999999999996</v>
       </c>
       <c r="L20">
-        <v>7024610.0992000001</v>
+        <v>7006900.6945999898</v>
       </c>
       <c r="M20">
-        <v>4739176.84469999</v>
+        <v>4735679.5045999996</v>
       </c>
       <c r="N20">
-        <v>0.26519999999999999</v>
+        <v>0.26869999999999999</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
@@ -3240,16 +3240,16 @@
         <v>446</v>
       </c>
       <c r="K21">
-        <v>6.8003</v>
+        <v>6.8277999999999999</v>
       </c>
       <c r="L21">
-        <v>7666704.7692</v>
+        <v>7617075.6844999902</v>
       </c>
       <c r="M21">
-        <v>5141774.2081000004</v>
+        <v>5098734.0138999997</v>
       </c>
       <c r="N21">
-        <v>0.1517</v>
+        <v>0.16259999999999999</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
@@ -3313,16 +3313,16 @@
         <v>3611.7</v>
       </c>
       <c r="K24">
-        <v>4.5190000000000001</v>
+        <v>4.4086999999999996</v>
       </c>
       <c r="L24">
-        <v>3772238.8974000001</v>
+        <v>3722339.142</v>
       </c>
       <c r="M24">
-        <v>2431785.8969999999</v>
+        <v>2407725.95299999</v>
       </c>
       <c r="N24">
-        <v>0.78949999999999998</v>
+        <v>0.79500000000000004</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
@@ -3351,16 +3351,16 @@
         <v>401.3</v>
       </c>
       <c r="K25">
-        <v>7.9043000000000001</v>
+        <v>7.7796000000000003</v>
       </c>
       <c r="L25">
-        <v>7003919.6168</v>
+        <v>6963352.8272000002</v>
       </c>
       <c r="M25">
-        <v>4737312.6979999999</v>
+        <v>4714035.4066000003</v>
       </c>
       <c r="N25">
-        <v>0.26939999999999997</v>
+        <v>0.2777</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
@@ -3389,16 +3389,16 @@
         <v>446</v>
       </c>
       <c r="K26">
-        <v>6.8898999999999999</v>
+        <v>6.8105999999999902</v>
       </c>
       <c r="L26">
-        <v>7656707.4136999901</v>
+        <v>7619603.5614999998</v>
       </c>
       <c r="M26">
-        <v>5137810.8506999901</v>
+        <v>5109145.7723000003</v>
       </c>
       <c r="N26">
-        <v>0.15379999999999999</v>
+        <v>0.16199999999999901</v>
       </c>
     </row>
   </sheetData>
@@ -3411,7 +3411,7 @@
   <dimension ref="B2:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3595,9 +3595,6 @@
       <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
       <c r="J9" t="s">
         <v>2</v>
       </c>
@@ -3640,16 +3637,16 @@
         <v>152537.4</v>
       </c>
       <c r="K10">
-        <v>0.60449999999999904</v>
+        <v>0.60399999999999898</v>
       </c>
       <c r="L10">
-        <v>1774.1815999999999</v>
+        <v>1771.8401999999901</v>
       </c>
       <c r="M10">
-        <v>1160.3926999999901</v>
+        <v>1159.27529999999</v>
       </c>
       <c r="N10">
-        <v>0.62629999999999997</v>
+        <v>0.62729999999999997</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -3678,16 +3675,16 @@
         <v>16948.599999999999</v>
       </c>
       <c r="K11">
-        <v>0.61470000000000002</v>
+        <v>0.61370000000000002</v>
       </c>
       <c r="L11">
-        <v>1895.10489999999</v>
+        <v>1893.9047</v>
       </c>
       <c r="M11">
-        <v>1193.6968999999999</v>
+        <v>1193.6670999999999</v>
       </c>
       <c r="N11">
-        <v>0.57309999999999905</v>
+        <v>0.57349999999999901</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -3716,13 +3713,13 @@
         <v>18832</v>
       </c>
       <c r="K12">
-        <v>0.60409999999999997</v>
+        <v>0.60729999999999995</v>
       </c>
       <c r="L12">
-        <v>1957.3897999999999</v>
+        <v>1957.7544</v>
       </c>
       <c r="M12">
-        <v>1205.9322999999999</v>
+        <v>1206.3689999999999</v>
       </c>
       <c r="N12">
         <v>0.55130000000000001</v>
@@ -3760,9 +3757,6 @@
       <c r="G19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" t="s">
-        <v>23</v>
-      </c>
       <c r="J19" t="s">
         <v>2</v>
       </c>
@@ -3805,16 +3799,16 @@
         <v>152537.4</v>
       </c>
       <c r="K20">
-        <v>0.60560000000000003</v>
+        <v>0.60370000000000001</v>
       </c>
       <c r="L20">
-        <v>1774.1351</v>
+        <v>1771.4305999999999</v>
       </c>
       <c r="M20">
-        <v>1160.4704999999999</v>
+        <v>1158.8183999999901</v>
       </c>
       <c r="N20">
-        <v>0.62619999999999998</v>
+        <v>0.62739999999999996</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
@@ -3843,16 +3837,16 @@
         <v>16948.599999999999</v>
       </c>
       <c r="K21">
-        <v>0.6149</v>
+        <v>0.61349999999999905</v>
       </c>
       <c r="L21">
-        <v>1891.6841999999899</v>
+        <v>1890.8679</v>
       </c>
       <c r="M21">
-        <v>1193.5409</v>
+        <v>1193.6813</v>
       </c>
       <c r="N21">
-        <v>0.57469999999999899</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
@@ -3881,16 +3875,16 @@
         <v>18832</v>
       </c>
       <c r="K22">
-        <v>0.60529999999999995</v>
+        <v>0.60539999999999905</v>
       </c>
       <c r="L22">
-        <v>1958.5450000000001</v>
+        <v>1957.6081999999999</v>
       </c>
       <c r="M22">
-        <v>1206.4586999999899</v>
+        <v>1206.4852000000001</v>
       </c>
       <c r="N22">
-        <v>0.55079999999999996</v>
+        <v>0.55120000000000002</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
@@ -3912,24 +3906,6 @@
       <c r="G24" t="s">
         <v>6</v>
       </c>
-      <c r="I24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" t="s">
-        <v>2</v>
-      </c>
-      <c r="K24" t="s">
-        <v>3</v>
-      </c>
-      <c r="L24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M24" t="s">
-        <v>5</v>
-      </c>
-      <c r="N24" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
@@ -3950,24 +3926,6 @@
       <c r="G25">
         <v>0.62660000000000005</v>
       </c>
-      <c r="I25" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25">
-        <v>152537.4</v>
-      </c>
-      <c r="K25">
-        <v>0.60489999999999999</v>
-      </c>
-      <c r="L25">
-        <v>1773.5389</v>
-      </c>
-      <c r="M25">
-        <v>1160.2295999999999</v>
-      </c>
-      <c r="N25">
-        <v>0.62660000000000005</v>
-      </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -3988,24 +3946,6 @@
       <c r="G26">
         <v>0.57230000000000003</v>
       </c>
-      <c r="I26" t="s">
-        <v>8</v>
-      </c>
-      <c r="J26">
-        <v>16948.599999999999</v>
-      </c>
-      <c r="K26">
-        <v>0.61509999999999998</v>
-      </c>
-      <c r="L26">
-        <v>1896.537</v>
-      </c>
-      <c r="M26">
-        <v>1194.0726</v>
-      </c>
-      <c r="N26">
-        <v>0.57230000000000003</v>
-      </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
@@ -4024,24 +3964,6 @@
         <v>1206.4589000000001</v>
       </c>
       <c r="G27">
-        <v>0.55130000000000001</v>
-      </c>
-      <c r="I27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27">
-        <v>18832</v>
-      </c>
-      <c r="K27">
-        <v>0.60470000000000002</v>
-      </c>
-      <c r="L27">
-        <v>1957.6405</v>
-      </c>
-      <c r="M27">
-        <v>1206.4589000000001</v>
-      </c>
-      <c r="N27">
         <v>0.55130000000000001</v>
       </c>
     </row>

</xml_diff>